<commit_message>
Added:  Tests/test_DataDrivenIteration.py  Utilities/get_ddt()  get_ddt_iteration()  Config/file for ddt
</commit_message>
<xml_diff>
--- a/POMFramework_POC/TestData/TDexcel_SkillBoard.xlsx
+++ b/POMFramework_POC/TestData/TDexcel_SkillBoard.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sindh\PycharmProjects\POMFramework_POC\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC8D1B8C-EA55-4E54-9810-B2C967C0DDD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A2EF9DF-A795-4DB7-8CE6-2BCB6067069C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4452" yWindow="3360" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -51,61 +51,61 @@
     <t>TestCase</t>
   </si>
   <si>
+    <t>tc_2</t>
+  </si>
+  <si>
+    <t>tc_3</t>
+  </si>
+  <si>
+    <t>tc_4</t>
+  </si>
+  <si>
+    <t>firstname</t>
+  </si>
+  <si>
+    <t>lastname</t>
+  </si>
+  <si>
+    <t>sindhu</t>
+  </si>
+  <si>
+    <t>boston</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>test_1</t>
+  </si>
+  <si>
+    <t>test1_emal@gmail.com</t>
+  </si>
+  <si>
+    <t>test2_emal@gmail.com</t>
+  </si>
+  <si>
+    <t>test3_emal@gmail.com</t>
+  </si>
+  <si>
+    <t>test4_emal@gmail.com</t>
+  </si>
+  <si>
+    <t>test5_emal@gmail.com</t>
+  </si>
+  <si>
+    <t>test6_emal@gmail.com</t>
+  </si>
+  <si>
+    <t>Test1!psw</t>
+  </si>
+  <si>
+    <t>Sign_Up</t>
+  </si>
+  <si>
     <t>tc_1</t>
   </si>
   <si>
-    <t>tc_2</t>
-  </si>
-  <si>
-    <t>tc_3</t>
-  </si>
-  <si>
-    <t>tc_4</t>
-  </si>
-  <si>
-    <t>tc_5</t>
-  </si>
-  <si>
     <t>tc_6</t>
-  </si>
-  <si>
-    <t>firstname</t>
-  </si>
-  <si>
-    <t>lastname</t>
-  </si>
-  <si>
-    <t>sindhu</t>
-  </si>
-  <si>
-    <t>boston</t>
-  </si>
-  <si>
-    <t>email</t>
-  </si>
-  <si>
-    <t>test_1</t>
-  </si>
-  <si>
-    <t>test1_emal@gmail.com</t>
-  </si>
-  <si>
-    <t>test2_emal@gmail.com</t>
-  </si>
-  <si>
-    <t>test3_emal@gmail.com</t>
-  </si>
-  <si>
-    <t>test4_emal@gmail.com</t>
-  </si>
-  <si>
-    <t>test5_emal@gmail.com</t>
-  </si>
-  <si>
-    <t>test6_emal@gmail.com</t>
-  </si>
-  <si>
-    <t>Test1!psw</t>
   </si>
 </sst>
 </file>
@@ -433,17 +433,17 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.28515625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -460,44 +460,44 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>18</v>
-      </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E2" s="1">
         <v>100036589</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="G2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>20</v>
-      </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>4</v>
@@ -506,24 +506,24 @@
         <v>5</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E3" s="1">
         <v>100036590</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>6</v>
@@ -532,24 +532,24 @@
         <v>5</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E4" s="1">
         <v>100036591</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>4</v>
@@ -558,24 +558,24 @@
         <v>5</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E5" s="1">
         <v>100036592</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>6</v>
@@ -584,24 +584,24 @@
         <v>5</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E6" s="1">
         <v>100036593</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>4</v>
@@ -610,19 +610,19 @@
         <v>5</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E7" s="1">
         <v>100036594</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added:  test_Signup_SkillBoard_DDT.py to execute ddt  Tests/test_DataDrivenIteration.py  Utilities/get_ddt()  get_ddt_iteration()  Config/file for ddt
</commit_message>
<xml_diff>
--- a/POMFramework_POC/TestData/TDexcel_SkillBoard.xlsx
+++ b/POMFramework_POC/TestData/TDexcel_SkillBoard.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sindh\PycharmProjects\POMFramework_POC\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A2EF9DF-A795-4DB7-8CE6-2BCB6067069C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C0CA369-A348-43D2-A4DC-8172C5EA0D20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6135" yWindow="3045" windowWidth="9405" windowHeight="6090" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="27">
-  <si>
-    <t>Region</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="37">
   <si>
     <t>username</t>
   </si>
@@ -36,76 +33,109 @@
     <t>password</t>
   </si>
   <si>
-    <t>policynumber</t>
-  </si>
-  <si>
-    <t>QA2</t>
-  </si>
-  <si>
-    <t>sindhuboston</t>
-  </si>
-  <si>
-    <t>preprod</t>
-  </si>
-  <si>
     <t>TestCase</t>
   </si>
   <si>
-    <t>tc_2</t>
-  </si>
-  <si>
-    <t>tc_3</t>
-  </si>
-  <si>
-    <t>tc_4</t>
-  </si>
-  <si>
     <t>firstname</t>
   </si>
   <si>
     <t>lastname</t>
   </si>
   <si>
-    <t>sindhu</t>
-  </si>
-  <si>
-    <t>boston</t>
-  </si>
-  <si>
     <t>email</t>
   </si>
   <si>
     <t>test_1</t>
   </si>
   <si>
-    <t>test1_emal@gmail.com</t>
-  </si>
-  <si>
-    <t>test2_emal@gmail.com</t>
-  </si>
-  <si>
-    <t>test3_emal@gmail.com</t>
-  </si>
-  <si>
-    <t>test4_emal@gmail.com</t>
-  </si>
-  <si>
-    <t>test5_emal@gmail.com</t>
-  </si>
-  <si>
-    <t>test6_emal@gmail.com</t>
-  </si>
-  <si>
     <t>Test1!psw</t>
   </si>
   <si>
     <t>Sign_Up</t>
   </si>
   <si>
-    <t>tc_1</t>
-  </si>
-  <si>
-    <t>tc_6</t>
+    <t>test_2</t>
+  </si>
+  <si>
+    <t>test_3</t>
+  </si>
+  <si>
+    <t>test_4</t>
+  </si>
+  <si>
+    <t>test_5</t>
+  </si>
+  <si>
+    <t>test_6</t>
+  </si>
+  <si>
+    <t>Test2!psw</t>
+  </si>
+  <si>
+    <t>Test3!psw</t>
+  </si>
+  <si>
+    <t>Test4!psw</t>
+  </si>
+  <si>
+    <t>Test5!psw</t>
+  </si>
+  <si>
+    <t>Test6!psw</t>
+  </si>
+  <si>
+    <t>snd_1</t>
+  </si>
+  <si>
+    <t>snd_2</t>
+  </si>
+  <si>
+    <t>snd_3</t>
+  </si>
+  <si>
+    <t>snd_4</t>
+  </si>
+  <si>
+    <t>snd_5</t>
+  </si>
+  <si>
+    <t>snd_6</t>
+  </si>
+  <si>
+    <t>boston_1</t>
+  </si>
+  <si>
+    <t>boston_2</t>
+  </si>
+  <si>
+    <t>boston_3</t>
+  </si>
+  <si>
+    <t>boston_4</t>
+  </si>
+  <si>
+    <t>boston_5</t>
+  </si>
+  <si>
+    <t>boston_6</t>
+  </si>
+  <si>
+    <t>test1_emal@gml.com</t>
+  </si>
+  <si>
+    <t>test2_emal@gml.com</t>
+  </si>
+  <si>
+    <t>test3_emal@gml.com</t>
+  </si>
+  <si>
+    <t>test4_emal@gml.com</t>
+  </si>
+  <si>
+    <t>test5_emal@gml.com</t>
+  </si>
+  <si>
+    <t>test6_emal@gml.com</t>
   </si>
 </sst>
 </file>
@@ -147,9 +177,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -430,22 +461,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.28515625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -454,175 +485,133 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E2" s="1">
-        <v>100036589</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>17</v>
+      <c r="F2" s="2" t="s">
+        <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E3" s="1">
-        <v>100036590</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4" s="1">
-        <v>100036591</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5" s="1">
-        <v>100036592</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="1">
-        <v>100036593</v>
-      </c>
-      <c r="F6" s="1" t="s">
+      <c r="E6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="C7" s="1" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E7" s="1">
-        <v>100036594</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
TD correction in test_LoginSkillBoard.py:
</commit_message>
<xml_diff>
--- a/POMFramework_POC/TestData/TDexcel_SkillBoard.xlsx
+++ b/POMFramework_POC/TestData/TDexcel_SkillBoard.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sindh\PycharmProjects\POMFramework_POC\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C0CA369-A348-43D2-A4DC-8172C5EA0D20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5C10814-8EDD-488A-85CF-82AE53E98C7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6135" yWindow="3045" windowWidth="9405" windowHeight="6090" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>username</t>
   </si>
@@ -51,9 +51,6 @@
     <t>Test1!psw</t>
   </si>
   <si>
-    <t>Sign_Up</t>
-  </si>
-  <si>
     <t>test_2</t>
   </si>
   <si>
@@ -136,6 +133,24 @@
   </si>
   <si>
     <t>test6_emal@gml.com</t>
+  </si>
+  <si>
+    <t>tc_1</t>
+  </si>
+  <si>
+    <t>tc_3</t>
+  </si>
+  <si>
+    <t>tc_4</t>
+  </si>
+  <si>
+    <t>tc_5</t>
+  </si>
+  <si>
+    <t>tc_6</t>
+  </si>
+  <si>
+    <t>test_signup_on_skillboard</t>
   </si>
 </sst>
 </file>
@@ -177,10 +192,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -464,17 +478,18 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.33203125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -494,9 +509,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>8</v>
+        <v>36</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>6</v>
@@ -505,113 +520,113 @@
         <v>7</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="1" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="1" t="s">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="1" t="s">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F6" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="1" t="s">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F7" t="s">
         <v>35</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modified SkillBoard test names moved the cancel button click after validations screenshot gets added in the report on a validation failure test executions continue to cover other validations, in case of assertion E
</commit_message>
<xml_diff>
--- a/POMFramework_POC/TestData/TDexcel_SkillBoard.xlsx
+++ b/POMFramework_POC/TestData/TDexcel_SkillBoard.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sindh\PycharmProjects\POMFramework_POC\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5C10814-8EDD-488A-85CF-82AE53E98C7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B0A850D-5962-410C-8C0B-BB9210A6B372}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -66,9 +66,6 @@
     <t>test_6</t>
   </si>
   <si>
-    <t>Test2!psw</t>
-  </si>
-  <si>
     <t>Test3!psw</t>
   </si>
   <si>
@@ -151,6 +148,9 @@
   </si>
   <si>
     <t>test_signup_on_skillboard</t>
+  </si>
+  <si>
+    <t>test2!psw</t>
   </si>
 </sst>
 </file>
@@ -478,18 +478,18 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.28515625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -509,9 +509,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>6</v>
@@ -520,113 +520,113 @@
         <v>7</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>13</v>
+        <v>41</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>